<commit_message>
Updated Groups excel sheet and regeenrated mappings
</commit_message>
<xml_diff>
--- a/mappings/veris-1.3.7/input/groups/xlsx/veris-1_3_7-mappings-groups_v12.xlsx
+++ b/mappings/veris-1.3.7/input/groups/xlsx/veris-1_3_7-mappings-groups_v12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26216"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbergeron\Documents\_VERIS II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15E1B5CF-874C-4EDD-B4CB-6419AFADBB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4511672C-3348-4ECD-8C60-F2081DDD664E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50520" yWindow="285" windowWidth="25440" windowHeight="15390" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
+    <workbookView xWindow="-50520" yWindow="285" windowWidth="25440" windowHeight="15390" firstSheet="1" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="252">
   <si>
     <t>ATT&amp;CK Integration into VERIS</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>Darkhotel</t>
+  </si>
+  <si>
+    <t>G0009</t>
+  </si>
+  <si>
+    <t>Deep Panda</t>
   </si>
   <si>
     <t>G0035</t>
@@ -1297,9 +1303,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6282965B-FDFE-4AAA-82BD-42D9A17F5C8F}">
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
@@ -1621,7 +1629,7 @@
       </c>
     </row>
     <row r="38" spans="2:3">
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C38" t="s">
@@ -1629,7 +1637,7 @@
       </c>
     </row>
     <row r="39" spans="2:3">
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C39" t="s">
@@ -1645,7 +1653,7 @@
       </c>
     </row>
     <row r="41" spans="2:3">
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C41" t="s">
@@ -1720,7 +1728,7 @@
       <c r="B50" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1728,7 +1736,7 @@
       <c r="B51" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="8" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1752,7 +1760,7 @@
       <c r="B54" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1760,7 +1768,7 @@
       <c r="B55" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="8" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1768,7 +1776,7 @@
       <c r="B56" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1776,7 +1784,7 @@
       <c r="B57" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="9" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1792,7 +1800,7 @@
       <c r="B59" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1816,7 +1824,7 @@
       <c r="B62" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="8" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1824,7 +1832,7 @@
       <c r="B63" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1928,7 +1936,7 @@
       <c r="B76" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="8" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1936,7 +1944,7 @@
       <c r="B77" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C77" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1944,7 +1952,7 @@
       <c r="B78" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="9" t="s">
         <v>166</v>
       </c>
     </row>
@@ -1960,7 +1968,7 @@
       <c r="B80" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C80" t="s">
         <v>170</v>
       </c>
     </row>
@@ -1976,7 +1984,7 @@
       <c r="B82" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="8" t="s">
         <v>174</v>
       </c>
     </row>
@@ -1984,7 +1992,7 @@
       <c r="B83" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="C83" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1992,7 +2000,7 @@
       <c r="B84" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="8" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2000,7 +2008,7 @@
       <c r="B85" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C85" s="8" t="s">
+      <c r="C85" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2024,58 +2032,58 @@
       <c r="B88" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C88" s="11" t="s">
+      <c r="C88" s="8" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" t="s">
+      <c r="B89" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="C89" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>189</v>
+      </c>
+      <c r="B90" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
-      <c r="B90" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C90" t="s">
-        <v>189</v>
-      </c>
-    </row>
     <row r="91" spans="1:3">
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C91" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="B92" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="B92" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C92" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="B93" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C93" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="7" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2089,18 +2097,18 @@
     </row>
     <row r="96" spans="1:3">
       <c r="B96" s="3" t="s">
-        <v>69</v>
+        <v>198</v>
       </c>
       <c r="C96" t="s">
-        <v>70</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97" spans="2:3">
       <c r="B97" s="3" t="s">
-        <v>198</v>
+        <v>71</v>
       </c>
       <c r="C97" t="s">
-        <v>199</v>
+        <v>72</v>
       </c>
     </row>
     <row r="98" spans="2:3">
@@ -2160,7 +2168,7 @@
       </c>
     </row>
     <row r="105" spans="2:3">
-      <c r="B105" s="6" t="s">
+      <c r="B105" s="3" t="s">
         <v>214</v>
       </c>
       <c r="C105" t="s">
@@ -2168,7 +2176,7 @@
       </c>
     </row>
     <row r="106" spans="2:3">
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="6" t="s">
         <v>216</v>
       </c>
       <c r="C106" t="s">
@@ -2176,7 +2184,7 @@
       </c>
     </row>
     <row r="107" spans="2:3">
-      <c r="B107" s="6" t="s">
+      <c r="B107" s="3" t="s">
         <v>218</v>
       </c>
       <c r="C107" t="s">
@@ -2185,50 +2193,50 @@
     </row>
     <row r="108" spans="2:3">
       <c r="B108" s="6" t="s">
-        <v>91</v>
+        <v>220</v>
       </c>
       <c r="C108" t="s">
-        <v>92</v>
+        <v>221</v>
       </c>
     </row>
     <row r="109" spans="2:3">
       <c r="B109" s="6" t="s">
-        <v>220</v>
+        <v>93</v>
       </c>
       <c r="C109" t="s">
-        <v>221</v>
+        <v>94</v>
       </c>
     </row>
     <row r="110" spans="2:3">
       <c r="B110" s="6" t="s">
-        <v>95</v>
+        <v>222</v>
       </c>
       <c r="C110" t="s">
-        <v>96</v>
+        <v>223</v>
       </c>
     </row>
     <row r="111" spans="2:3">
       <c r="B111" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C111" s="8" t="s">
-        <v>223</v>
+        <v>97</v>
+      </c>
+      <c r="C111" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="112" spans="2:3">
       <c r="B112" s="6" t="s">
-        <v>131</v>
+        <v>224</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>132</v>
+        <v>225</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="B113" s="6" t="s">
-        <v>224</v>
+        <v>133</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>225</v>
+        <v>134</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2240,58 +2248,58 @@
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="8" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="B116" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C116" s="8" t="s">
-        <v>148</v>
+      <c r="B116" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C116" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="B117" s="6" t="s">
-        <v>230</v>
+        <v>149</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>231</v>
+        <v>150</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="B118" s="6" t="s">
-        <v>157</v>
+        <v>232</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>158</v>
+        <v>233</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="B119" s="6" t="s">
-        <v>232</v>
+        <v>159</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>233</v>
+        <v>160</v>
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="8" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="B121" s="6" t="s">
+      <c r="B121" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C121" s="8" t="s">
+      <c r="C121" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2304,85 +2312,93 @@
       </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="B123" s="3" t="s">
+      <c r="B123" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="8" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" t="s">
+      <c r="B124" s="3" t="s">
         <v>242</v>
+      </c>
+      <c r="C124" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B94" r:id="rId1" xr:uid="{09732BDD-83D7-4E93-84DB-1BFEE5FEFBFB}"/>
-    <hyperlink ref="B91" r:id="rId2" xr:uid="{9A12EC6C-281E-45B1-AC28-A34D3C14140B}"/>
-    <hyperlink ref="B95" r:id="rId3" xr:uid="{925F4635-90F1-4BE8-86F2-C8F6D0A9C0FD}"/>
-    <hyperlink ref="B96" r:id="rId4" xr:uid="{A8E90F17-E38C-4874-BE8F-B67F6975000B}"/>
-    <hyperlink ref="B97" r:id="rId5" xr:uid="{02C55956-6BF3-4DD3-8CAF-E30590F18187}"/>
-    <hyperlink ref="B98" r:id="rId6" xr:uid="{B7753C61-1C4C-4672-940F-3D3148FD9726}"/>
-    <hyperlink ref="B33" r:id="rId7" xr:uid="{015B48B1-D998-4743-AF9E-5B7505DFDC10}"/>
-    <hyperlink ref="B34" r:id="rId8" xr:uid="{86A67FEB-477E-4C27-ADFB-F2E248D93BE6}"/>
-    <hyperlink ref="B35" r:id="rId9" xr:uid="{711D7F9D-2CED-44F2-AEB2-AAD48FCCC6AF}"/>
-    <hyperlink ref="B36" r:id="rId10" xr:uid="{224243C2-8A1F-4DC1-9A01-3353D31897A1}"/>
-    <hyperlink ref="B37" r:id="rId11" xr:uid="{A5ECDF18-1D53-46B5-8488-6FB6B42BB7FE}"/>
-    <hyperlink ref="B39" r:id="rId12" xr:uid="{9E7D8D41-1F6A-45B1-844C-6FCAFB9B7144}"/>
-    <hyperlink ref="B40" r:id="rId13" xr:uid="{6A054EA0-FA03-48EA-B973-7534261E38A6}"/>
-    <hyperlink ref="B42" r:id="rId14" xr:uid="{4581EE3A-3684-42E4-9F11-B63759E904A7}"/>
-    <hyperlink ref="B45" r:id="rId15" xr:uid="{9238E2C2-D36C-4302-B5F7-2A8D37B144A4}"/>
-    <hyperlink ref="B47" r:id="rId16" xr:uid="{47860278-9CEF-4BD5-891E-B186BD3D2F7C}"/>
-    <hyperlink ref="B48" r:id="rId17" xr:uid="{E7E35011-B2E5-4A64-ACCF-A5891BB69747}"/>
-    <hyperlink ref="B49" r:id="rId18" xr:uid="{3BDD6B22-535B-4A28-BE5A-2C35E24F9E63}"/>
-    <hyperlink ref="B51" r:id="rId19" xr:uid="{B46DA7B8-2A31-4FE4-B5B5-2E7F1F40B407}"/>
-    <hyperlink ref="B52" r:id="rId20" xr:uid="{5225494F-4BD5-4B22-A1E0-7A5A391DB4AC}"/>
-    <hyperlink ref="B53" r:id="rId21" xr:uid="{002C482B-A44D-4280-8447-B9818C165A95}"/>
-    <hyperlink ref="B55" r:id="rId22" xr:uid="{51CC0E33-F9FC-42C3-89D4-D3C937E48F8E}"/>
-    <hyperlink ref="B57" r:id="rId23" xr:uid="{1BA5E7BB-42E3-4A26-88BA-59F42E73F36E}"/>
-    <hyperlink ref="B58" r:id="rId24" xr:uid="{A89248B9-DCF2-495F-B9A2-A6DECB9891DA}"/>
-    <hyperlink ref="B62" r:id="rId25" xr:uid="{07947366-A915-40EE-BCF1-9AD0C268FB84}"/>
-    <hyperlink ref="B76" r:id="rId26" xr:uid="{1C5DA79A-A9B2-47BB-9EAA-86E2CA18924C}"/>
-    <hyperlink ref="B78" r:id="rId27" xr:uid="{2EE67E1D-9A20-4BC2-826D-A8EB84829AD3}"/>
-    <hyperlink ref="B79" r:id="rId28" xr:uid="{8BFFB16B-CEF3-44E3-B020-F4A94E180DAE}"/>
-    <hyperlink ref="B82" r:id="rId29" xr:uid="{B059F175-9B1F-452E-AF24-75E58C60DBD4}"/>
-    <hyperlink ref="B84" r:id="rId30" xr:uid="{4179F2D9-CBA7-4BBE-9619-D557DE39BB0D}"/>
+    <hyperlink ref="B95" r:id="rId1" xr:uid="{09732BDD-83D7-4E93-84DB-1BFEE5FEFBFB}"/>
+    <hyperlink ref="B92" r:id="rId2" xr:uid="{9A12EC6C-281E-45B1-AC28-A34D3C14140B}"/>
+    <hyperlink ref="B96" r:id="rId3" xr:uid="{925F4635-90F1-4BE8-86F2-C8F6D0A9C0FD}"/>
+    <hyperlink ref="B97" r:id="rId4" xr:uid="{A8E90F17-E38C-4874-BE8F-B67F6975000B}"/>
+    <hyperlink ref="B98" r:id="rId5" xr:uid="{02C55956-6BF3-4DD3-8CAF-E30590F18187}"/>
+    <hyperlink ref="B99" r:id="rId6" xr:uid="{B7753C61-1C4C-4672-940F-3D3148FD9726}"/>
+    <hyperlink ref="B34" r:id="rId7" xr:uid="{015B48B1-D998-4743-AF9E-5B7505DFDC10}"/>
+    <hyperlink ref="B35" r:id="rId8" xr:uid="{86A67FEB-477E-4C27-ADFB-F2E248D93BE6}"/>
+    <hyperlink ref="B36" r:id="rId9" xr:uid="{711D7F9D-2CED-44F2-AEB2-AAD48FCCC6AF}"/>
+    <hyperlink ref="B37" r:id="rId10" xr:uid="{224243C2-8A1F-4DC1-9A01-3353D31897A1}"/>
+    <hyperlink ref="B38" r:id="rId11" xr:uid="{A5ECDF18-1D53-46B5-8488-6FB6B42BB7FE}"/>
+    <hyperlink ref="B40" r:id="rId12" xr:uid="{9E7D8D41-1F6A-45B1-844C-6FCAFB9B7144}"/>
+    <hyperlink ref="B41" r:id="rId13" xr:uid="{6A054EA0-FA03-48EA-B973-7534261E38A6}"/>
+    <hyperlink ref="B43" r:id="rId14" xr:uid="{4581EE3A-3684-42E4-9F11-B63759E904A7}"/>
+    <hyperlink ref="B46" r:id="rId15" xr:uid="{9238E2C2-D36C-4302-B5F7-2A8D37B144A4}"/>
+    <hyperlink ref="B48" r:id="rId16" xr:uid="{47860278-9CEF-4BD5-891E-B186BD3D2F7C}"/>
+    <hyperlink ref="B49" r:id="rId17" xr:uid="{E7E35011-B2E5-4A64-ACCF-A5891BB69747}"/>
+    <hyperlink ref="B50" r:id="rId18" xr:uid="{3BDD6B22-535B-4A28-BE5A-2C35E24F9E63}"/>
+    <hyperlink ref="B52" r:id="rId19" xr:uid="{B46DA7B8-2A31-4FE4-B5B5-2E7F1F40B407}"/>
+    <hyperlink ref="B53" r:id="rId20" xr:uid="{5225494F-4BD5-4B22-A1E0-7A5A391DB4AC}"/>
+    <hyperlink ref="B54" r:id="rId21" xr:uid="{002C482B-A44D-4280-8447-B9818C165A95}"/>
+    <hyperlink ref="B56" r:id="rId22" xr:uid="{51CC0E33-F9FC-42C3-89D4-D3C937E48F8E}"/>
+    <hyperlink ref="B58" r:id="rId23" xr:uid="{1BA5E7BB-42E3-4A26-88BA-59F42E73F36E}"/>
+    <hyperlink ref="B59" r:id="rId24" xr:uid="{A89248B9-DCF2-495F-B9A2-A6DECB9891DA}"/>
+    <hyperlink ref="B63" r:id="rId25" xr:uid="{07947366-A915-40EE-BCF1-9AD0C268FB84}"/>
+    <hyperlink ref="B77" r:id="rId26" xr:uid="{1C5DA79A-A9B2-47BB-9EAA-86E2CA18924C}"/>
+    <hyperlink ref="B79" r:id="rId27" xr:uid="{2EE67E1D-9A20-4BC2-826D-A8EB84829AD3}"/>
+    <hyperlink ref="B80" r:id="rId28" xr:uid="{8BFFB16B-CEF3-44E3-B020-F4A94E180DAE}"/>
+    <hyperlink ref="B83" r:id="rId29" xr:uid="{B059F175-9B1F-452E-AF24-75E58C60DBD4}"/>
+    <hyperlink ref="B85" r:id="rId30" xr:uid="{4179F2D9-CBA7-4BBE-9619-D557DE39BB0D}"/>
     <hyperlink ref="B14" r:id="rId31" xr:uid="{A9EE67DC-92B6-42F0-A39A-2C43084AB4D6}"/>
     <hyperlink ref="B15" r:id="rId32" xr:uid="{AFF279A3-AF87-41FC-A637-6DA15E1B518D}"/>
     <hyperlink ref="B16" r:id="rId33" xr:uid="{13E37386-203B-47D7-8E11-1BD672DED0DA}"/>
@@ -2396,65 +2412,65 @@
     <hyperlink ref="B25" r:id="rId41" xr:uid="{DBF7BB98-1DEF-4444-9FEF-C2A9720149AD}"/>
     <hyperlink ref="B26" r:id="rId42" xr:uid="{2A23F430-DA25-4E43-8330-ED7C91E70847}"/>
     <hyperlink ref="B28" r:id="rId43" xr:uid="{41706294-CB32-4BF6-A92E-EB9FA6809132}"/>
-    <hyperlink ref="B29" r:id="rId44" xr:uid="{3C8EC5CE-0772-4291-B7C3-EFEA6C73D338}"/>
-    <hyperlink ref="B30" r:id="rId45" xr:uid="{2A22A421-F17B-403E-9065-2043E7C0F6C1}"/>
-    <hyperlink ref="B31" r:id="rId46" xr:uid="{01EC1831-1B88-4B53-9218-7323CE7629E2}"/>
-    <hyperlink ref="B32" r:id="rId47" xr:uid="{2CEB6D94-0040-4FE7-AB97-E75FC96B2082}"/>
-    <hyperlink ref="B101" r:id="rId48" xr:uid="{54D5DCFA-9990-46CC-BCDA-0FF6480E728C}"/>
-    <hyperlink ref="B102" r:id="rId49" xr:uid="{89337EB2-5DDE-432A-B02F-F9F7C6434F3D}"/>
-    <hyperlink ref="B103" r:id="rId50" xr:uid="{7C032773-9D34-4789-97C9-A4C7ADC61F38}"/>
-    <hyperlink ref="B104" r:id="rId51" xr:uid="{D868BD0E-7506-4680-A467-5D083F54532A}"/>
-    <hyperlink ref="B106" r:id="rId52" xr:uid="{EBA005FF-63A2-4A57-B921-A0D36E842108}"/>
-    <hyperlink ref="B115" r:id="rId53" xr:uid="{11D17740-5592-4532-9E48-882F8A0D2371}"/>
-    <hyperlink ref="B120" r:id="rId54" xr:uid="{CEC0175B-B004-4D3B-83DF-CD083703F4F2}"/>
-    <hyperlink ref="B123" r:id="rId55" xr:uid="{B75C7993-0B7E-4FA8-BC7B-62AAD617C441}"/>
+    <hyperlink ref="B30" r:id="rId44" xr:uid="{3C8EC5CE-0772-4291-B7C3-EFEA6C73D338}"/>
+    <hyperlink ref="B31" r:id="rId45" xr:uid="{2A22A421-F17B-403E-9065-2043E7C0F6C1}"/>
+    <hyperlink ref="B32" r:id="rId46" xr:uid="{01EC1831-1B88-4B53-9218-7323CE7629E2}"/>
+    <hyperlink ref="B33" r:id="rId47" xr:uid="{2CEB6D94-0040-4FE7-AB97-E75FC96B2082}"/>
+    <hyperlink ref="B102" r:id="rId48" xr:uid="{54D5DCFA-9990-46CC-BCDA-0FF6480E728C}"/>
+    <hyperlink ref="B103" r:id="rId49" xr:uid="{89337EB2-5DDE-432A-B02F-F9F7C6434F3D}"/>
+    <hyperlink ref="B104" r:id="rId50" xr:uid="{7C032773-9D34-4789-97C9-A4C7ADC61F38}"/>
+    <hyperlink ref="B105" r:id="rId51" xr:uid="{D868BD0E-7506-4680-A467-5D083F54532A}"/>
+    <hyperlink ref="B107" r:id="rId52" xr:uid="{EBA005FF-63A2-4A57-B921-A0D36E842108}"/>
+    <hyperlink ref="B116" r:id="rId53" xr:uid="{11D17740-5592-4532-9E48-882F8A0D2371}"/>
+    <hyperlink ref="B121" r:id="rId54" xr:uid="{CEC0175B-B004-4D3B-83DF-CD083703F4F2}"/>
+    <hyperlink ref="B124" r:id="rId55" xr:uid="{B75C7993-0B7E-4FA8-BC7B-62AAD617C441}"/>
     <hyperlink ref="B2" r:id="rId56" xr:uid="{F4B6398E-5647-42B9-BCF6-83E7D25768D3}"/>
     <hyperlink ref="B3" r:id="rId57" xr:uid="{F404ED6C-50AA-4712-B0BD-06C63A1E10AA}"/>
     <hyperlink ref="B5" r:id="rId58" xr:uid="{9315A52A-425A-4342-8CE1-1CD4F09D96C3}"/>
     <hyperlink ref="B6" r:id="rId59" xr:uid="{8DA870EC-3162-4FA2-8816-6FC77406CDBB}"/>
-    <hyperlink ref="B100" r:id="rId60" xr:uid="{786C519F-DA59-4683-8107-9AA63D996940}"/>
-    <hyperlink ref="B99" r:id="rId61" xr:uid="{7DE273E4-3EB5-4A6F-8B96-D2F25337DA5C}"/>
-    <hyperlink ref="B111" r:id="rId62" xr:uid="{D4F2A2DA-E39E-4DCC-A89C-AC1CD70D6D4C}"/>
-    <hyperlink ref="B112" r:id="rId63" xr:uid="{B3482C4B-771F-4E3D-8378-CE8241C356D1}"/>
-    <hyperlink ref="B113" r:id="rId64" xr:uid="{644A71CC-BC95-4E97-8F55-2609D562882D}"/>
-    <hyperlink ref="B114" r:id="rId65" xr:uid="{7337C350-B53F-4C67-8258-D73D9E977123}"/>
-    <hyperlink ref="B116" r:id="rId66" xr:uid="{63B58D37-CC78-417E-B394-5FDBFF4716E3}"/>
-    <hyperlink ref="B117" r:id="rId67" xr:uid="{0906D5E4-B147-4421-8D20-829BF3523B2F}"/>
-    <hyperlink ref="B118" r:id="rId68" xr:uid="{B07C349E-DA3A-419C-80F9-A5C803D22CD4}"/>
-    <hyperlink ref="B119" r:id="rId69" xr:uid="{9E53E2C9-3ED7-49C3-8B8D-49D7862F9674}"/>
-    <hyperlink ref="B121" r:id="rId70" xr:uid="{B4FD28C5-D99E-46D0-BC38-9A1C827F99C1}"/>
+    <hyperlink ref="B101" r:id="rId60" xr:uid="{786C519F-DA59-4683-8107-9AA63D996940}"/>
+    <hyperlink ref="B100" r:id="rId61" xr:uid="{7DE273E4-3EB5-4A6F-8B96-D2F25337DA5C}"/>
+    <hyperlink ref="B112" r:id="rId62" xr:uid="{D4F2A2DA-E39E-4DCC-A89C-AC1CD70D6D4C}"/>
+    <hyperlink ref="B113" r:id="rId63" xr:uid="{B3482C4B-771F-4E3D-8378-CE8241C356D1}"/>
+    <hyperlink ref="B114" r:id="rId64" xr:uid="{644A71CC-BC95-4E97-8F55-2609D562882D}"/>
+    <hyperlink ref="B115" r:id="rId65" xr:uid="{7337C350-B53F-4C67-8258-D73D9E977123}"/>
+    <hyperlink ref="B117" r:id="rId66" xr:uid="{63B58D37-CC78-417E-B394-5FDBFF4716E3}"/>
+    <hyperlink ref="B118" r:id="rId67" xr:uid="{0906D5E4-B147-4421-8D20-829BF3523B2F}"/>
+    <hyperlink ref="B119" r:id="rId68" xr:uid="{B07C349E-DA3A-419C-80F9-A5C803D22CD4}"/>
+    <hyperlink ref="B120" r:id="rId69" xr:uid="{9E53E2C9-3ED7-49C3-8B8D-49D7862F9674}"/>
+    <hyperlink ref="B122" r:id="rId70" xr:uid="{B4FD28C5-D99E-46D0-BC38-9A1C827F99C1}"/>
     <hyperlink ref="B4" r:id="rId71" display="https://attack.mitre.org/groups/G0138" xr:uid="{3E753C92-3AF3-4C3F-B315-C697EF10AEE8}"/>
     <hyperlink ref="B8" r:id="rId72" display="https://attack.mitre.org/groups/G0005" xr:uid="{3D717BB6-86C4-4973-A82C-4D1C98999868}"/>
     <hyperlink ref="B9" r:id="rId73" display="https://attack.mitre.org/groups/G0023" xr:uid="{FA4F573F-FC65-4CBA-87D1-9BF0B4CA95B7}"/>
-    <hyperlink ref="B50" r:id="rId74" xr:uid="{A00231B1-2CBC-44EB-BBFF-C39D26AD584E}"/>
-    <hyperlink ref="B54" r:id="rId75" xr:uid="{62AF05E0-B33D-4DC8-971A-7A17E4271F24}"/>
-    <hyperlink ref="B56" r:id="rId76" xr:uid="{EBA69880-2F36-44C3-9B12-242CD42B609B}"/>
-    <hyperlink ref="B59" r:id="rId77" xr:uid="{A8EE7D5B-9845-4FD8-8141-0AB10871AD29}"/>
-    <hyperlink ref="B60" r:id="rId78" xr:uid="{142CF992-8BD1-43CD-840F-9D83C040738C}"/>
-    <hyperlink ref="B61" r:id="rId79" xr:uid="{8F810D73-3571-46AF-820E-E8E978479F22}"/>
-    <hyperlink ref="B63" r:id="rId80" xr:uid="{75F28F51-74A4-46FF-A526-BFB05B775565}"/>
-    <hyperlink ref="B64" r:id="rId81" xr:uid="{D02A05B1-62A2-4373-BD9A-0F2FA923C023}"/>
-    <hyperlink ref="B65" r:id="rId82" xr:uid="{3289C029-CAEB-4B8D-AE8A-0762A33D98F2}"/>
-    <hyperlink ref="B66" r:id="rId83" xr:uid="{983ED5AB-8E75-4780-A9F9-034404FDF030}"/>
-    <hyperlink ref="B67" r:id="rId84" xr:uid="{A9CFB1BF-779D-4E9C-BF98-BB5A656DF6E9}"/>
-    <hyperlink ref="B68" r:id="rId85" xr:uid="{8BA9CB52-7D78-4A22-AD37-CFEC38768BAC}"/>
-    <hyperlink ref="B69" r:id="rId86" xr:uid="{BD9B0832-420C-4ACD-895A-3E19987447F5}"/>
-    <hyperlink ref="B70" r:id="rId87" xr:uid="{989EAA78-C5E7-4037-BEA7-BF47B11DF2D8}"/>
-    <hyperlink ref="B71" r:id="rId88" xr:uid="{FE795333-D111-48FE-8C64-296C28CE1F73}"/>
-    <hyperlink ref="B72" r:id="rId89" xr:uid="{12691F9F-3902-47C1-9371-44119B9E5B3C}"/>
-    <hyperlink ref="B73" r:id="rId90" xr:uid="{D70D7E4F-4D01-4FB7-BB60-3AD5B3570E87}"/>
-    <hyperlink ref="B74" r:id="rId91" xr:uid="{3D54D5B1-D305-42E4-A794-CD65B3AA783D}"/>
-    <hyperlink ref="B75" r:id="rId92" xr:uid="{B09CDBF4-54DF-4EB0-93DD-7FDDE5A052D0}"/>
-    <hyperlink ref="B77" r:id="rId93" xr:uid="{5D6180B9-F947-49EE-A7B0-5DA93D7DC833}"/>
-    <hyperlink ref="B80" r:id="rId94" xr:uid="{32FF8CEE-18AF-42D7-BDB6-366BB8408451}"/>
-    <hyperlink ref="B81" r:id="rId95" xr:uid="{E6213DD7-48DC-4310-ABA5-4D434E7E5E1A}"/>
-    <hyperlink ref="B83" r:id="rId96" xr:uid="{0F43F625-BFE0-4A44-9B5D-9FA76BD1AF72}"/>
-    <hyperlink ref="B122" r:id="rId97" xr:uid="{8C56CAB3-514B-4380-9004-C8DE7AF092F3}"/>
-    <hyperlink ref="B85" r:id="rId98" xr:uid="{EF7F890A-06C9-492B-A417-A7871136EE1F}"/>
-    <hyperlink ref="B86" r:id="rId99" xr:uid="{CE0795B4-822C-45F1-BC1E-760B13A2B8C5}"/>
-    <hyperlink ref="B87" r:id="rId100" xr:uid="{E771425F-4152-4283-95F2-853C3167761A}"/>
-    <hyperlink ref="B88" r:id="rId101" xr:uid="{ADBA5944-D9C5-48FA-9408-695F7BD368F0}"/>
-    <hyperlink ref="B89" r:id="rId102" display="https://attack.mitre.org/groups/G0138" xr:uid="{44245983-7863-4A50-AA4A-9E440B059A12}"/>
+    <hyperlink ref="B51" r:id="rId74" xr:uid="{A00231B1-2CBC-44EB-BBFF-C39D26AD584E}"/>
+    <hyperlink ref="B55" r:id="rId75" xr:uid="{62AF05E0-B33D-4DC8-971A-7A17E4271F24}"/>
+    <hyperlink ref="B57" r:id="rId76" xr:uid="{EBA69880-2F36-44C3-9B12-242CD42B609B}"/>
+    <hyperlink ref="B60" r:id="rId77" xr:uid="{A8EE7D5B-9845-4FD8-8141-0AB10871AD29}"/>
+    <hyperlink ref="B61" r:id="rId78" xr:uid="{142CF992-8BD1-43CD-840F-9D83C040738C}"/>
+    <hyperlink ref="B62" r:id="rId79" xr:uid="{8F810D73-3571-46AF-820E-E8E978479F22}"/>
+    <hyperlink ref="B64" r:id="rId80" xr:uid="{75F28F51-74A4-46FF-A526-BFB05B775565}"/>
+    <hyperlink ref="B65" r:id="rId81" xr:uid="{D02A05B1-62A2-4373-BD9A-0F2FA923C023}"/>
+    <hyperlink ref="B66" r:id="rId82" xr:uid="{3289C029-CAEB-4B8D-AE8A-0762A33D98F2}"/>
+    <hyperlink ref="B67" r:id="rId83" xr:uid="{983ED5AB-8E75-4780-A9F9-034404FDF030}"/>
+    <hyperlink ref="B68" r:id="rId84" xr:uid="{A9CFB1BF-779D-4E9C-BF98-BB5A656DF6E9}"/>
+    <hyperlink ref="B69" r:id="rId85" xr:uid="{8BA9CB52-7D78-4A22-AD37-CFEC38768BAC}"/>
+    <hyperlink ref="B70" r:id="rId86" xr:uid="{BD9B0832-420C-4ACD-895A-3E19987447F5}"/>
+    <hyperlink ref="B71" r:id="rId87" xr:uid="{989EAA78-C5E7-4037-BEA7-BF47B11DF2D8}"/>
+    <hyperlink ref="B72" r:id="rId88" xr:uid="{FE795333-D111-48FE-8C64-296C28CE1F73}"/>
+    <hyperlink ref="B73" r:id="rId89" xr:uid="{12691F9F-3902-47C1-9371-44119B9E5B3C}"/>
+    <hyperlink ref="B74" r:id="rId90" xr:uid="{D70D7E4F-4D01-4FB7-BB60-3AD5B3570E87}"/>
+    <hyperlink ref="B75" r:id="rId91" xr:uid="{3D54D5B1-D305-42E4-A794-CD65B3AA783D}"/>
+    <hyperlink ref="B76" r:id="rId92" xr:uid="{B09CDBF4-54DF-4EB0-93DD-7FDDE5A052D0}"/>
+    <hyperlink ref="B78" r:id="rId93" xr:uid="{5D6180B9-F947-49EE-A7B0-5DA93D7DC833}"/>
+    <hyperlink ref="B81" r:id="rId94" xr:uid="{32FF8CEE-18AF-42D7-BDB6-366BB8408451}"/>
+    <hyperlink ref="B82" r:id="rId95" xr:uid="{E6213DD7-48DC-4310-ABA5-4D434E7E5E1A}"/>
+    <hyperlink ref="B84" r:id="rId96" xr:uid="{0F43F625-BFE0-4A44-9B5D-9FA76BD1AF72}"/>
+    <hyperlink ref="B123" r:id="rId97" xr:uid="{8C56CAB3-514B-4380-9004-C8DE7AF092F3}"/>
+    <hyperlink ref="B86" r:id="rId98" xr:uid="{EF7F890A-06C9-492B-A417-A7871136EE1F}"/>
+    <hyperlink ref="B87" r:id="rId99" xr:uid="{CE0795B4-822C-45F1-BC1E-760B13A2B8C5}"/>
+    <hyperlink ref="B88" r:id="rId100" xr:uid="{E771425F-4152-4283-95F2-853C3167761A}"/>
+    <hyperlink ref="B89" r:id="rId101" xr:uid="{ADBA5944-D9C5-48FA-9408-695F7BD368F0}"/>
+    <hyperlink ref="B90" r:id="rId102" display="https://attack.mitre.org/groups/G0138" xr:uid="{44245983-7863-4A50-AA4A-9E440B059A12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2470,25 +2486,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date_x0020__x0026__x0020_Time xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <ProjectNum xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <TotalCost xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <Participants xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ec3e3de1-934b-464b-893a-587ae869df79" xsi:nil="true"/>
-    <MasterListID xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <ProjectName xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-    <CostPer xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010052D8A6B6F9FE2E45B0EDBAAD5FAF1312" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7022bf91ca57a9626808ed15fdcbfbd6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xmlns:ns3="ec3e3de1-934b-464b-893a-587ae869df79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d11a2dadb3f3bef5d5d1fdbc6ca57c91" ns2:_="" ns3:_="">
     <xsd:import namespace="0ca01121-da18-407e-86a0-e0ab1b6c7d8c"/>
@@ -2787,14 +2784,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date_x0020__x0026__x0020_Time xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <ProjectNum xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <TotalCost xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <Participants xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ec3e3de1-934b-464b-893a-587ae869df79" xsi:nil="true"/>
+    <MasterListID xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <ProjectName xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+    <CostPer xmlns="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C05FA04D-3647-4F57-90F3-FA0A2E1CF7AC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C12CA17C-B5EA-4F79-A387-28384A9BE73D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{697EDC42-9C5C-463C-A7CA-B1F330E8878B}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{697EDC42-9C5C-463C-A7CA-B1F330E8878B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C12CA17C-B5EA-4F79-A387-28384A9BE73D}"/>
 </file>
</xml_diff>